<commit_message>
Merge the powerpoint file
</commit_message>
<xml_diff>
--- a/PCB/02 Plans & Actuals/2.3_Risk & Issue/Risk Tracker.xlsx
+++ b/PCB/02 Plans & Actuals/2.3_Risk & Issue/Risk Tracker.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="10920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25460" windowHeight="12560"/>
   </bookViews>
   <sheets>
     <sheet name="Risk Plan" sheetId="1" r:id="rId1"/>
@@ -20,25 +20,30 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Risk Plan'!$A$3:$I$6</definedName>
-    <definedName name="a">'[5]Project Summary'!#REF!</definedName>
-    <definedName name="Code_Size">'[3]Project Summary'!#REF!</definedName>
-    <definedName name="Des_Size">'[3]Project Summary'!#REF!</definedName>
-    <definedName name="Maint_Size">'[3]Project Summary'!#REF!</definedName>
-    <definedName name="NSD_Size">'[3]Project Summary'!#REF!</definedName>
-    <definedName name="Phases">'[2]Validation Lists'!$E$2:$E$11</definedName>
+    <definedName name="a">'[1]Project Summary'!#REF!</definedName>
+    <definedName name="Code_Size">'[2]Project Summary'!#REF!</definedName>
+    <definedName name="Des_Size">'[2]Project Summary'!#REF!</definedName>
+    <definedName name="Maint_Size">'[2]Project Summary'!#REF!</definedName>
+    <definedName name="NSD_Size">'[2]Project Summary'!#REF!</definedName>
+    <definedName name="Phases">'[3]Validation Lists'!$E$2:$E$11</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Risk Plan'!$A$1:$L$22</definedName>
-    <definedName name="q">'[5]Project Summary'!#REF!</definedName>
-    <definedName name="Req_Size">'[3]Project Summary'!#REF!</definedName>
-    <definedName name="Resp">'[1]Validation Lists'!$C$2:$C$4</definedName>
-    <definedName name="Slippage_Reason">'[2]Validation Lists'!$D$2:$D$19</definedName>
-    <definedName name="Status">'[1]Validation Lists'!$B$2:$B$7</definedName>
-    <definedName name="Test_Size">'[3]Project Summary'!#REF!</definedName>
-    <definedName name="wp_size">'[4]Peer Review File Upload'!$J$23:$J$503</definedName>
-    <definedName name="wp_type">'[4]Peer Review File Upload'!$F$23:$F$503</definedName>
-    <definedName name="wp_unit">'[4]Peer Review File Upload'!$I$23:$I$503</definedName>
+    <definedName name="q">'[1]Project Summary'!#REF!</definedName>
+    <definedName name="Req_Size">'[2]Project Summary'!#REF!</definedName>
+    <definedName name="Resp">'[4]Validation Lists'!$C$2:$C$4</definedName>
+    <definedName name="Slippage_Reason">'[3]Validation Lists'!$D$2:$D$19</definedName>
+    <definedName name="Status">'[4]Validation Lists'!$B$2:$B$7</definedName>
+    <definedName name="Test_Size">'[2]Project Summary'!#REF!</definedName>
+    <definedName name="wp_size">'[5]Peer Review File Upload'!$J$23:$J$503</definedName>
+    <definedName name="wp_type">'[5]Peer Review File Upload'!$F$23:$F$503</definedName>
+    <definedName name="wp_unit">'[5]Peer Review File Upload'!$I$23:$I$503</definedName>
     <definedName name="wss">'[6]Peer Review File Upload'!$J$23:$J$503</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -236,11 +241,6 @@
 </t>
   </si>
   <si>
-    <t>1. Use LIGHT document.
-2. Use more chart, table and graph to documentate our design.
-3. Ask others for review.</t>
-  </si>
-  <si>
     <t>All Team Members</t>
   </si>
   <si>
@@ -276,6 +276,13 @@
   <si>
     <t>2015-08-18 
 (for 1#. U.S.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Use LIGHT document.
+2. Use more chart, table and graph to documentate our design.
+3. Ask others for review.
+</t>
+    <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -383,251 +390,251 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -635,23 +642,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -787,6 +794,21 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -814,24 +836,9 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -912,212 +919,20 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Validation Lists"/>
-      <sheetName val="Notes"/>
-      <sheetName val="M-DV (Mthly Progress)"/>
-      <sheetName val="M-DV (Phase End)"/>
-      <sheetName val="Mthly Charts"/>
-      <sheetName val="PM_metrics99"/>
+      <sheetName val="Project Summary"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>Inactive</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>COSL</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>Hold</v>
-          </cell>
-          <cell r="C3" t="str">
-            <v>Customer</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>Completed</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>NA</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>Active</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v>Canceled</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>NA</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Validation Lists"/>
-      <sheetName val="Notes"/>
-      <sheetName val="M-DV (Mthly Progress)"/>
-      <sheetName val="M-DV (Phase End)"/>
-      <sheetName val="Mthly Charts"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="D2" t="str">
-            <v>Cust1. Chg in Priorities</v>
-          </cell>
-          <cell r="E2" t="str">
-            <v>*</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="D3" t="str">
-            <v>Cust2. Chg Impl Date</v>
-          </cell>
-          <cell r="E3" t="str">
-            <v xml:space="preserve">Initiation </v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="D4" t="str">
-            <v>Cust3. Chg Specs</v>
-          </cell>
-          <cell r="E4" t="str">
-            <v>Definition : RS</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5" t="str">
-            <v>Devl1. Infrastructure</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>Definition : FS</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6" t="str">
-            <v>Devl2. Underestimated</v>
-          </cell>
-          <cell r="E6" t="str">
-            <v>Technical Design : DES</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>Devl3. Prob Discovered</v>
-          </cell>
-          <cell r="E7" t="str">
-            <v>Construction : CON</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>Devl4. Staff Availability</v>
-          </cell>
-          <cell r="E8" t="str">
-            <v>Construction : TST</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9" t="str">
-            <v>Devl5. Prod Problems</v>
-          </cell>
-          <cell r="E9" t="str">
-            <v>Validation : UAT</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="D10" t="str">
-            <v>Devl6. Vendor Delay</v>
-          </cell>
-          <cell r="E10" t="str">
-            <v>Implementation</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11" t="str">
-            <v>Devl8. Approvals Coord</v>
-          </cell>
-          <cell r="E11" t="str">
-            <v>Post Implementation</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12" t="str">
-            <v>Devl9. External Coord</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13" t="str">
-            <v>UAT1. Delay in Testing</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14" t="str">
-            <v>UAT2. User Availability</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15" t="str">
-            <v>UAT3. Region Availability</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16" t="str">
-            <v>UAT4. Prob Disc in UAT</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="D17" t="str">
-            <v>UAT5. Pending Rev Approval</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="D18" t="str">
-            <v>No Response</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="D19" t="str">
-            <v>Other</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Project Summary"/>
@@ -1159,8 +974,34 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Validation Lists"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Validation Lists"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Instructions"/>
@@ -1232,47 +1073,8 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Project Summary"/>
-      <sheetName val="Metrics Thesholds"/>
-      <sheetName val="Metrics Chart"/>
-      <sheetName val="Metrics Summary"/>
-      <sheetName val="Metrics Data Inputs"/>
-      <sheetName val="Control Chart"/>
-      <sheetName val="Module End Metrics"/>
-      <sheetName val="Defects (Monthly)"/>
-      <sheetName val="Project End Metrics "/>
-      <sheetName val="Control Panel"/>
-      <sheetName val="PDB Sheet"/>
-      <sheetName val="Terms in Metrics"/>
-      <sheetName val="Document Control History"/>
-      <sheetName val="Template Control History "/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Instructions"/>
@@ -1668,31 +1470,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L33" sqref="L33"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" style="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="22" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="22" customWidth="1"/>
     <col min="4" max="4" width="41" style="22" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" style="22" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="22" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="22" customWidth="1"/>
-    <col min="12" max="12" width="32.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="23" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.83203125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="22" customWidth="1"/>
+    <col min="12" max="12" width="32.5" style="22" customWidth="1"/>
     <col min="13" max="16384" width="3" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="3" customFormat="1" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="3" customFormat="1" ht="19" customHeight="1" thickBot="1">
       <c r="A1" s="2"/>
       <c r="E1" s="2"/>
       <c r="U1" s="4">
@@ -1702,30 +1504,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="52" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="55" t="s">
+      <c r="H2" s="58"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="56"/>
-      <c r="L2" s="57"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="62"/>
       <c r="U2" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="5" customFormat="1" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="5" customFormat="1" ht="34.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>45</v>
       </c>
@@ -1767,7 +1569,7 @@
       </c>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:22" s="15" customFormat="1" ht="129" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" s="15" customFormat="1" ht="105" thickTop="1">
       <c r="A4" s="30">
         <v>1</v>
       </c>
@@ -1787,12 +1589,12 @@
         <v>47</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="58">
+        <v>58</v>
+      </c>
+      <c r="I4" s="49">
         <v>42238</v>
       </c>
       <c r="J4" s="33" t="s">
@@ -1802,14 +1604,14 @@
         <v>55</v>
       </c>
       <c r="L4" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U4" s="16">
         <v>5</v>
       </c>
       <c r="V4" s="16"/>
     </row>
-    <row r="5" spans="1:22" s="15" customFormat="1" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" s="15" customFormat="1" ht="91">
       <c r="A5" s="30">
         <v>2</v>
       </c>
@@ -1829,13 +1631,13 @@
         <v>53</v>
       </c>
       <c r="G5" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="53" t="s">
         <v>66</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="62" t="s">
-        <v>67</v>
       </c>
       <c r="J5" s="33" t="s">
         <v>47</v>
@@ -1844,14 +1646,14 @@
         <v>53</v>
       </c>
       <c r="L5" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U5" s="16">
         <v>5</v>
       </c>
       <c r="V5" s="16"/>
     </row>
-    <row r="6" spans="1:22" s="15" customFormat="1" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" s="15" customFormat="1" ht="78">
       <c r="A6" s="30">
         <v>3</v>
       </c>
@@ -1862,7 +1664,7 @@
         <v>49</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>55</v>
@@ -1871,12 +1673,12 @@
         <v>53</v>
       </c>
       <c r="G6" s="43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" s="59">
+        <v>58</v>
+      </c>
+      <c r="I6" s="50">
         <v>42238</v>
       </c>
       <c r="J6" s="44" t="s">
@@ -1886,12 +1688,12 @@
         <v>56</v>
       </c>
       <c r="L6" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U6" s="16"/>
       <c r="V6" s="16"/>
     </row>
-    <row r="7" spans="1:22" s="15" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" s="15" customFormat="1" ht="65">
       <c r="A7" s="30">
         <v>4</v>
       </c>
@@ -1911,13 +1713,13 @@
         <v>55</v>
       </c>
       <c r="G7" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="I7" s="50" t="s">
         <v>59</v>
-      </c>
-      <c r="I7" s="59" t="s">
-        <v>60</v>
       </c>
       <c r="J7" s="44" t="s">
         <v>56</v>
@@ -1926,10 +1728,10 @@
         <v>55</v>
       </c>
       <c r="L7" s="34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="15" customFormat="1">
       <c r="A8" s="30">
         <v>5</v>
       </c>
@@ -1940,14 +1742,14 @@
       <c r="F8" s="35"/>
       <c r="G8" s="43"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="59"/>
+      <c r="I8" s="50"/>
       <c r="J8" s="44"/>
       <c r="K8" s="17"/>
       <c r="L8" s="34"/>
       <c r="U8" s="16"/>
       <c r="V8" s="16"/>
     </row>
-    <row r="9" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" s="15" customFormat="1">
       <c r="A9" s="30">
         <v>6</v>
       </c>
@@ -1958,12 +1760,12 @@
       <c r="F9" s="35"/>
       <c r="G9" s="43"/>
       <c r="H9" s="18"/>
-      <c r="I9" s="59"/>
+      <c r="I9" s="50"/>
       <c r="J9" s="44"/>
       <c r="K9" s="17"/>
       <c r="L9" s="34"/>
     </row>
-    <row r="10" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" s="15" customFormat="1">
       <c r="A10" s="30">
         <v>7</v>
       </c>
@@ -1974,12 +1776,12 @@
       <c r="F10" s="35"/>
       <c r="G10" s="43"/>
       <c r="H10" s="18"/>
-      <c r="I10" s="59"/>
+      <c r="I10" s="50"/>
       <c r="J10" s="44"/>
       <c r="K10" s="17"/>
       <c r="L10" s="34"/>
     </row>
-    <row r="11" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" s="15" customFormat="1">
       <c r="A11" s="30">
         <v>8</v>
       </c>
@@ -1990,12 +1792,12 @@
       <c r="F11" s="35"/>
       <c r="G11" s="43"/>
       <c r="H11" s="18"/>
-      <c r="I11" s="59"/>
+      <c r="I11" s="50"/>
       <c r="J11" s="44"/>
       <c r="K11" s="17"/>
       <c r="L11" s="34"/>
     </row>
-    <row r="12" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" s="15" customFormat="1">
       <c r="A12" s="30">
         <v>9</v>
       </c>
@@ -2006,12 +1808,12 @@
       <c r="F12" s="35"/>
       <c r="G12" s="44"/>
       <c r="H12" s="18"/>
-      <c r="I12" s="60"/>
+      <c r="I12" s="51"/>
       <c r="J12" s="44"/>
       <c r="K12" s="17"/>
       <c r="L12" s="34"/>
     </row>
-    <row r="13" spans="1:22" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" s="15" customFormat="1" ht="14" thickBot="1">
       <c r="A13" s="30">
         <v>10</v>
       </c>
@@ -2022,157 +1824,157 @@
       <c r="F13" s="39"/>
       <c r="G13" s="45"/>
       <c r="H13" s="37"/>
-      <c r="I13" s="61"/>
+      <c r="I13" s="52"/>
       <c r="J13" s="45"/>
       <c r="K13" s="38"/>
       <c r="L13" s="48"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22">
       <c r="A15" s="20"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22">
       <c r="A16" s="20"/>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" s="20"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="20"/>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="20"/>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="20"/>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="20"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="20"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" s="20"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" s="20"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" s="20"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" s="20"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" s="20"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" s="20"/>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" s="20"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" s="20"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" s="20"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" s="20"/>
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" s="20"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" s="20"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" s="20"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" s="20"/>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" s="20"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" s="20"/>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" s="20"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" s="20"/>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" s="20"/>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42" s="20"/>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3">
       <c r="A43" s="20"/>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
@@ -2202,13 +2004,18 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="8" scale="84" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="84" orientation="landscape"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;"Arial,加粗"&amp;K000000VEL team&amp;C&amp;K000000&amp;D&amp;R&amp;K000000Page &amp;N</oddFooter>
   </headerFooter>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="12" max="1048575" man="1"/>
   </colBreaks>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2216,19 +2023,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q38"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="75" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A5" zoomScale="75" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.33203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="6.28515625" style="1"/>
+    <col min="1" max="16384" width="6.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="12.75" customHeight="1">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -2249,7 +2056,7 @@
       <c r="P4" s="26"/>
       <c r="Q4" s="26"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17">
       <c r="A5" s="26"/>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
@@ -2268,7 +2075,7 @@
       <c r="P5" s="26"/>
       <c r="Q5" s="26"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17">
       <c r="A6" s="26"/>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
@@ -2287,185 +2094,185 @@
       <c r="P6" s="26"/>
       <c r="Q6" s="26"/>
     </row>
-    <row r="7" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="14">
       <c r="A7" s="27" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="28"/>
     </row>
-    <row r="8" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="14">
       <c r="A8" s="29" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="28"/>
     </row>
-    <row r="9" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="14">
       <c r="A9" s="29" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="28"/>
     </row>
-    <row r="10" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="14">
       <c r="A10" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="28"/>
     </row>
-    <row r="11" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="14">
       <c r="A11" s="29"/>
       <c r="B11" s="28"/>
     </row>
-    <row r="12" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="14">
       <c r="A12" s="27" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="28"/>
     </row>
-    <row r="13" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="14">
       <c r="A13" s="29" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="28"/>
     </row>
-    <row r="14" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="14">
       <c r="A14" s="29" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="28"/>
     </row>
-    <row r="15" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="14">
       <c r="A15" s="29" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="28"/>
     </row>
-    <row r="16" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="14">
       <c r="A16" s="29"/>
       <c r="B16" s="28"/>
     </row>
-    <row r="17" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="14">
       <c r="A17" s="27" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="28"/>
     </row>
-    <row r="18" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="14">
       <c r="A18" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="28"/>
     </row>
-    <row r="19" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="14">
       <c r="A19" s="29" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="28"/>
     </row>
-    <row r="20" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="14">
       <c r="A20" s="29" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="28"/>
     </row>
-    <row r="21" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="14">
       <c r="A21" s="29" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="28"/>
     </row>
-    <row r="22" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="14">
       <c r="A22" s="29"/>
       <c r="B22" s="28"/>
     </row>
-    <row r="23" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="14">
       <c r="A23" s="27" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="28"/>
     </row>
-    <row r="24" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="14">
       <c r="A24" s="29" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="28"/>
     </row>
-    <row r="25" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="14">
       <c r="A25" s="29" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="28"/>
     </row>
-    <row r="26" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="14">
       <c r="A26" s="29" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="28"/>
     </row>
-    <row r="27" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="14">
       <c r="A27" s="29" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="28"/>
     </row>
-    <row r="28" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="14">
       <c r="A28" s="29" t="s">
         <v>43</v>
       </c>
       <c r="B28" s="28"/>
     </row>
-    <row r="29" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="14">
       <c r="A29" s="29" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="28"/>
     </row>
-    <row r="30" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="14">
       <c r="A30" s="29" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="28"/>
     </row>
-    <row r="31" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="14">
       <c r="A31" s="29"/>
       <c r="B31" s="28"/>
     </row>
-    <row r="32" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="14">
       <c r="A32" s="27" t="s">
         <v>32</v>
       </c>
       <c r="B32" s="28"/>
     </row>
-    <row r="33" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="14">
       <c r="A33" s="29" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="28"/>
     </row>
-    <row r="34" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="14">
       <c r="A34" s="29" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="28"/>
     </row>
-    <row r="35" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="14">
       <c r="A35" s="29" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="28"/>
     </row>
-    <row r="36" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="14">
       <c r="A36" s="29" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="28"/>
     </row>
-    <row r="37" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="14">
       <c r="A37" s="29" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="28"/>
     </row>
-    <row r="38" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="14">
       <c r="A38" s="29" t="s">
         <v>38</v>
       </c>
@@ -2478,5 +2285,10 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;"Arial,加粗"&amp;K000000VEL team&amp;C&amp;K000000&amp;D&amp;R&amp;K000000Page &amp;N</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>